<commit_message>
Dec2024 Add .gitignore, update database URLs, and enhance transaction models and controllers
</commit_message>
<xml_diff>
--- a/STEP6Calculated Cashflows.xlsx
+++ b/STEP6Calculated Cashflows.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="36">
   <si>
     <t>bank_account_key</t>
   </si>
@@ -483,7 +483,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -517,19 +517,19 @@
         <v>7</v>
       </c>
       <c r="B2" s="2">
-        <v>45444</v>
+        <v>45536</v>
       </c>
       <c r="C2" s="2">
-        <v>45473</v>
+        <v>45565</v>
       </c>
       <c r="D2">
-        <v>894.8</v>
+        <v>1144.8</v>
       </c>
       <c r="E2">
-        <v>7599.39</v>
+        <v>10383.79</v>
       </c>
       <c r="F2">
-        <v>7599.39</v>
+        <v>10383.79</v>
       </c>
       <c r="G2" t="s">
         <v>34</v>
@@ -540,19 +540,19 @@
         <v>7</v>
       </c>
       <c r="B3" s="2">
-        <v>45474</v>
+        <v>45566</v>
       </c>
       <c r="C3" s="2">
-        <v>45504</v>
+        <v>45596</v>
       </c>
       <c r="D3">
-        <v>494.8</v>
+        <v>1169.8</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>8094.190000000001</v>
+        <v>11553.59</v>
       </c>
       <c r="G3" t="s">
         <v>35</v>
@@ -560,25 +560,25 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2">
-        <v>45505</v>
+        <v>45536</v>
       </c>
       <c r="C4" s="2">
-        <v>45535</v>
+        <v>45565</v>
       </c>
       <c r="D4">
-        <v>-805.2</v>
+        <v>-772.88</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>4796.49</v>
       </c>
       <c r="F4">
-        <v>7288.990000000001</v>
+        <v>4796.49</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -586,65 +586,65 @@
         <v>8</v>
       </c>
       <c r="B5" s="2">
-        <v>45444</v>
+        <v>45566</v>
       </c>
       <c r="C5" s="2">
-        <v>45473</v>
+        <v>45596</v>
       </c>
       <c r="D5">
-        <v>1026.07</v>
+        <v>554.88</v>
       </c>
       <c r="E5">
-        <v>7217.23</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>7217.23</v>
+        <v>5351.37</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2">
-        <v>45474</v>
+        <v>45536</v>
       </c>
       <c r="C6" s="2">
-        <v>45504</v>
+        <v>45565</v>
       </c>
       <c r="D6">
-        <v>-823.9299999999999</v>
+        <v>1223.03</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>10017.96</v>
       </c>
       <c r="F6">
-        <v>6393.299999999999</v>
+        <v>10017.96</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2">
-        <v>45505</v>
+        <v>45566</v>
       </c>
       <c r="C7" s="2">
-        <v>45535</v>
+        <v>45596</v>
       </c>
       <c r="D7">
-        <v>-823.9299999999999</v>
+        <v>1223.03</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>5569.369999999999</v>
+        <v>11240.99</v>
       </c>
       <c r="G7" t="s">
         <v>35</v>
@@ -652,22 +652,22 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2">
-        <v>45444</v>
+        <v>45536</v>
       </c>
       <c r="C8" s="2">
-        <v>45473</v>
+        <v>45565</v>
       </c>
       <c r="D8">
-        <v>723.03</v>
+        <v>98.52</v>
       </c>
       <c r="E8">
-        <v>6448.87</v>
+        <v>6543.22</v>
       </c>
       <c r="F8">
-        <v>6448.87</v>
+        <v>6543.22</v>
       </c>
       <c r="G8" t="s">
         <v>34</v>
@@ -675,22 +675,22 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2">
-        <v>45474</v>
+        <v>45566</v>
       </c>
       <c r="C9" s="2">
-        <v>45504</v>
+        <v>45596</v>
       </c>
       <c r="D9">
-        <v>1123.03</v>
+        <v>1972.52</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>7571.9</v>
+        <v>8515.74</v>
       </c>
       <c r="G9" t="s">
         <v>35</v>
@@ -698,68 +698,68 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2">
-        <v>45505</v>
+        <v>45536</v>
       </c>
       <c r="C10" s="2">
-        <v>45535</v>
+        <v>45565</v>
       </c>
       <c r="D10">
-        <v>-801.97</v>
+        <v>1134.37</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>9254.049999999999</v>
       </c>
       <c r="F10">
-        <v>6769.929999999999</v>
+        <v>9254.049999999999</v>
       </c>
       <c r="G10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>45444</v>
+        <v>45566</v>
       </c>
       <c r="C11" s="2">
-        <v>45473</v>
+        <v>45596</v>
       </c>
       <c r="D11">
-        <v>-786.48</v>
+        <v>181.73</v>
       </c>
       <c r="E11">
-        <v>3899.52</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>3899.52</v>
+        <v>9435.779999999999</v>
       </c>
       <c r="G11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>45474</v>
+        <v>45597</v>
       </c>
       <c r="C12" s="2">
-        <v>45504</v>
+        <v>45626</v>
       </c>
       <c r="D12">
-        <v>3331.66</v>
+        <v>-675.63</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>7231.18</v>
+        <v>8760.15</v>
       </c>
       <c r="G12" t="s">
         <v>35</v>
@@ -767,91 +767,91 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>45505</v>
+        <v>45536</v>
       </c>
       <c r="C13" s="2">
-        <v>45535</v>
+        <v>45565</v>
       </c>
       <c r="D13">
-        <v>-786.48</v>
+        <v>1218.98</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>10537.9</v>
       </c>
       <c r="F13">
-        <v>6444.700000000001</v>
+        <v>10537.9</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2">
-        <v>45444</v>
+        <v>45566</v>
       </c>
       <c r="C14" s="2">
-        <v>45473</v>
+        <v>45596</v>
       </c>
       <c r="D14">
-        <v>834.37</v>
+        <v>1218.98</v>
       </c>
       <c r="E14">
-        <v>5966.22</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>5966.22</v>
+        <v>11756.88</v>
       </c>
       <c r="G14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2">
-        <v>45474</v>
+        <v>45536</v>
       </c>
       <c r="C15" s="2">
-        <v>45504</v>
+        <v>45565</v>
       </c>
       <c r="D15">
-        <v>1184.37</v>
+        <v>150.03</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>3261.52</v>
       </c>
       <c r="F15">
-        <v>7150.59</v>
+        <v>3261.52</v>
       </c>
       <c r="G15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B16" s="2">
-        <v>45505</v>
+        <v>45566</v>
       </c>
       <c r="C16" s="2">
-        <v>45535</v>
+        <v>45596</v>
       </c>
       <c r="D16">
-        <v>-675.63</v>
+        <v>150.03</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>6474.96</v>
+        <v>3411.55</v>
       </c>
       <c r="G16" t="s">
         <v>35</v>
@@ -859,22 +859,22 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B17" s="2">
-        <v>45444</v>
+        <v>45536</v>
       </c>
       <c r="C17" s="2">
-        <v>45473</v>
+        <v>45565</v>
       </c>
       <c r="D17">
-        <v>-582.02</v>
+        <v>-1444.66</v>
       </c>
       <c r="E17">
-        <v>7180.96</v>
+        <v>15261.69</v>
       </c>
       <c r="F17">
-        <v>7180.96</v>
+        <v>15261.69</v>
       </c>
       <c r="G17" t="s">
         <v>34</v>
@@ -882,22 +882,22 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B18" s="2">
-        <v>45474</v>
+        <v>45566</v>
       </c>
       <c r="C18" s="2">
-        <v>45504</v>
+        <v>45596</v>
       </c>
       <c r="D18">
-        <v>918.98</v>
+        <v>3856.25</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>8099.940000000001</v>
+        <v>19117.94</v>
       </c>
       <c r="G18" t="s">
         <v>35</v>
@@ -905,91 +905,91 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B19" s="2">
-        <v>45505</v>
+        <v>45536</v>
       </c>
       <c r="C19" s="2">
-        <v>45535</v>
+        <v>45565</v>
       </c>
       <c r="D19">
-        <v>-531.02</v>
+        <v>2651.62</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>12931.56</v>
       </c>
       <c r="F19">
-        <v>7568.92</v>
+        <v>12931.56</v>
       </c>
       <c r="G19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B20" s="2">
-        <v>45444</v>
+        <v>45566</v>
       </c>
       <c r="C20" s="2">
-        <v>45473</v>
+        <v>45596</v>
       </c>
       <c r="D20">
-        <v>150.02</v>
+        <v>-38.38</v>
       </c>
       <c r="E20">
-        <v>2811.44</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>2811.44</v>
+        <v>12893.18</v>
       </c>
       <c r="G20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B21" s="2">
-        <v>45474</v>
+        <v>45536</v>
       </c>
       <c r="C21" s="2">
-        <v>45504</v>
+        <v>45565</v>
       </c>
       <c r="D21">
-        <v>150.03</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>1965.73</v>
       </c>
       <c r="F21">
-        <v>2961.47</v>
+        <v>1965.73</v>
       </c>
       <c r="G21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B22" s="2">
-        <v>45444</v>
+        <v>45536</v>
       </c>
       <c r="C22" s="2">
-        <v>45473</v>
+        <v>45565</v>
       </c>
       <c r="D22">
-        <v>2408.35</v>
+        <v>0.02</v>
       </c>
       <c r="E22">
-        <v>14129.15</v>
+        <v>1723.5</v>
       </c>
       <c r="F22">
-        <v>14129.15</v>
+        <v>1723.5</v>
       </c>
       <c r="G22" t="s">
         <v>34</v>
@@ -997,22 +997,22 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B23" s="2">
-        <v>45474</v>
+        <v>45566</v>
       </c>
       <c r="C23" s="2">
-        <v>45504</v>
+        <v>45596</v>
       </c>
       <c r="D23">
-        <v>2201.84</v>
+        <v>0.01</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23">
-        <v>16330.99</v>
+        <v>1723.51</v>
       </c>
       <c r="G23" t="s">
         <v>35</v>
@@ -1020,45 +1020,45 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B24" s="2">
-        <v>45505</v>
+        <v>45139</v>
       </c>
       <c r="C24" s="2">
-        <v>45535</v>
+        <v>45169</v>
       </c>
       <c r="D24">
-        <v>-1113.16</v>
+        <v>-900</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>7579.48</v>
       </c>
       <c r="F24">
-        <v>15217.83</v>
+        <v>7579.48</v>
       </c>
       <c r="G24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B25" s="2">
-        <v>45444</v>
+        <v>45536</v>
       </c>
       <c r="C25" s="2">
-        <v>45473</v>
+        <v>45565</v>
       </c>
       <c r="D25">
-        <v>955.12</v>
+        <v>1602.39</v>
       </c>
       <c r="E25">
-        <v>7813.53</v>
+        <v>13971.89</v>
       </c>
       <c r="F25">
-        <v>7813.53</v>
+        <v>13971.89</v>
       </c>
       <c r="G25" t="s">
         <v>34</v>
@@ -1066,22 +1066,22 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B26" s="2">
-        <v>45474</v>
+        <v>45566</v>
       </c>
       <c r="C26" s="2">
-        <v>45504</v>
+        <v>45596</v>
       </c>
       <c r="D26">
-        <v>3104.79</v>
+        <v>1597.41</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
       <c r="F26">
-        <v>10918.32</v>
+        <v>15569.3</v>
       </c>
       <c r="G26" t="s">
         <v>35</v>
@@ -1089,68 +1089,68 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B27" s="2">
-        <v>45505</v>
+        <v>45536</v>
       </c>
       <c r="C27" s="2">
-        <v>45535</v>
+        <v>45565</v>
       </c>
       <c r="D27">
-        <v>-638.38</v>
+        <v>7432.61</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>25902.29</v>
       </c>
       <c r="F27">
-        <v>10279.94</v>
+        <v>25902.29</v>
       </c>
       <c r="G27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B28" s="2">
-        <v>45170</v>
+        <v>45566</v>
       </c>
       <c r="C28" s="2">
-        <v>45199</v>
+        <v>45596</v>
       </c>
       <c r="D28">
-        <v>825</v>
+        <v>379.0700000000001</v>
       </c>
       <c r="E28">
-        <v>1965.73</v>
+        <v>0</v>
       </c>
       <c r="F28">
-        <v>1965.73</v>
+        <v>26281.36</v>
       </c>
       <c r="G28" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B29" s="2">
-        <v>45444</v>
+        <v>45536</v>
       </c>
       <c r="C29" s="2">
-        <v>45473</v>
+        <v>45565</v>
       </c>
       <c r="D29">
-        <v>0.02</v>
+        <v>2237.59</v>
       </c>
       <c r="E29">
-        <v>1723.46</v>
+        <v>16890.32</v>
       </c>
       <c r="F29">
-        <v>1723.46</v>
+        <v>16890.32</v>
       </c>
       <c r="G29" t="s">
         <v>34</v>
@@ -1158,22 +1158,22 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B30" s="2">
-        <v>45474</v>
+        <v>45566</v>
       </c>
       <c r="C30" s="2">
-        <v>45504</v>
+        <v>45596</v>
       </c>
       <c r="D30">
-        <v>0.01</v>
+        <v>65.98000000000002</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30">
-        <v>1723.47</v>
+        <v>16956.3</v>
       </c>
       <c r="G30" t="s">
         <v>35</v>
@@ -1181,45 +1181,45 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B31" s="2">
-        <v>45139</v>
+        <v>45597</v>
       </c>
       <c r="C31" s="2">
-        <v>45169</v>
+        <v>45626</v>
       </c>
       <c r="D31">
-        <v>-900</v>
+        <v>-1383.06</v>
       </c>
       <c r="E31">
-        <v>7579.48</v>
+        <v>0</v>
       </c>
       <c r="F31">
-        <v>7579.48</v>
+        <v>15573.24</v>
       </c>
       <c r="G31" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B32" s="2">
-        <v>45444</v>
+        <v>45536</v>
       </c>
       <c r="C32" s="2">
-        <v>45473</v>
+        <v>45565</v>
       </c>
       <c r="D32">
-        <v>1552.34</v>
+        <v>181.94</v>
       </c>
       <c r="E32">
-        <v>8614.76</v>
+        <v>9722.58</v>
       </c>
       <c r="F32">
-        <v>8614.76</v>
+        <v>9722.58</v>
       </c>
       <c r="G32" t="s">
         <v>34</v>
@@ -1227,22 +1227,22 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B33" s="2">
-        <v>45474</v>
+        <v>45566</v>
       </c>
       <c r="C33" s="2">
-        <v>45504</v>
+        <v>45596</v>
       </c>
       <c r="D33">
-        <v>1752.36</v>
+        <v>2376.55</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
       <c r="F33">
-        <v>10367.12</v>
+        <v>12099.13</v>
       </c>
       <c r="G33" t="s">
         <v>35</v>
@@ -1250,22 +1250,22 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B34" s="2">
-        <v>45505</v>
+        <v>45597</v>
       </c>
       <c r="C34" s="2">
-        <v>45535</v>
+        <v>45626</v>
       </c>
       <c r="D34">
-        <v>-947.72</v>
+        <v>-1383.06</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34">
-        <v>9419.400000000001</v>
+        <v>10716.07</v>
       </c>
       <c r="G34" t="s">
         <v>35</v>
@@ -1273,22 +1273,22 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B35" s="2">
-        <v>45444</v>
+        <v>45536</v>
       </c>
       <c r="C35" s="2">
-        <v>45473</v>
+        <v>45565</v>
       </c>
       <c r="D35">
-        <v>-594.02</v>
+        <v>189.62</v>
       </c>
       <c r="E35">
-        <v>17400.94</v>
+        <v>998.63</v>
       </c>
       <c r="F35">
-        <v>17400.94</v>
+        <v>998.63</v>
       </c>
       <c r="G35" t="s">
         <v>34</v>
@@ -1296,22 +1296,22 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B36" s="2">
-        <v>45474</v>
+        <v>45566</v>
       </c>
       <c r="C36" s="2">
-        <v>45504</v>
+        <v>45596</v>
       </c>
       <c r="D36">
-        <v>846.3</v>
+        <v>-808.95</v>
       </c>
       <c r="E36">
         <v>0</v>
       </c>
       <c r="F36">
-        <v>18247.24</v>
+        <v>189.6799999999999</v>
       </c>
       <c r="G36" t="s">
         <v>35</v>
@@ -1319,22 +1319,22 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B37" s="2">
-        <v>45444</v>
+        <v>45474</v>
       </c>
       <c r="C37" s="2">
-        <v>45473</v>
+        <v>45504</v>
       </c>
       <c r="D37">
-        <v>-1383.06</v>
+        <v>-248</v>
       </c>
       <c r="E37">
-        <v>6604.32</v>
+        <v>3379.74</v>
       </c>
       <c r="F37">
-        <v>6604.32</v>
+        <v>3379.74</v>
       </c>
       <c r="G37" t="s">
         <v>34</v>
@@ -1342,45 +1342,45 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B38" s="2">
-        <v>45474</v>
+        <v>45536</v>
       </c>
       <c r="C38" s="2">
-        <v>45504</v>
+        <v>45565</v>
       </c>
       <c r="D38">
-        <v>5031.469999999999</v>
+        <v>-630.79</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>11160.5</v>
       </c>
       <c r="F38">
-        <v>11635.79</v>
+        <v>11160.5</v>
       </c>
       <c r="G38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B39" s="2">
-        <v>45505</v>
+        <v>45566</v>
       </c>
       <c r="C39" s="2">
-        <v>45535</v>
+        <v>45596</v>
       </c>
       <c r="D39">
-        <v>-1383.06</v>
+        <v>1306.21</v>
       </c>
       <c r="E39">
         <v>0</v>
       </c>
       <c r="F39">
-        <v>10252.73</v>
+        <v>12466.71</v>
       </c>
       <c r="G39" t="s">
         <v>35</v>
@@ -1388,22 +1388,22 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B40" s="2">
-        <v>45444</v>
+        <v>45536</v>
       </c>
       <c r="C40" s="2">
-        <v>45473</v>
+        <v>45565</v>
       </c>
       <c r="D40">
-        <v>1486.32</v>
+        <v>940.99</v>
       </c>
       <c r="E40">
-        <v>6851.35</v>
+        <v>12672.14</v>
       </c>
       <c r="F40">
-        <v>6851.35</v>
+        <v>12672.14</v>
       </c>
       <c r="G40" t="s">
         <v>34</v>
@@ -1411,22 +1411,22 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B41" s="2">
-        <v>45474</v>
+        <v>45566</v>
       </c>
       <c r="C41" s="2">
-        <v>45504</v>
+        <v>45596</v>
       </c>
       <c r="D41">
-        <v>1271.94</v>
+        <v>1230.99</v>
       </c>
       <c r="E41">
         <v>0</v>
       </c>
       <c r="F41">
-        <v>8123.290000000001</v>
+        <v>13903.13</v>
       </c>
       <c r="G41" t="s">
         <v>35</v>
@@ -1434,206 +1434,206 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B42" s="2">
-        <v>45505</v>
+        <v>45536</v>
       </c>
       <c r="C42" s="2">
-        <v>45535</v>
+        <v>45565</v>
       </c>
       <c r="D42">
-        <v>-1383.06</v>
+        <v>-71.53</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>377.92</v>
       </c>
       <c r="F42">
-        <v>6740.230000000001</v>
+        <v>377.92</v>
       </c>
       <c r="G42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B43" s="2">
-        <v>45444</v>
+        <v>45566</v>
       </c>
       <c r="C43" s="2">
-        <v>45473</v>
+        <v>45596</v>
       </c>
       <c r="D43">
-        <v>1656.05</v>
+        <v>-28.17</v>
       </c>
       <c r="E43">
-        <v>2426.91</v>
+        <v>0</v>
       </c>
       <c r="F43">
-        <v>2426.91</v>
+        <v>349.75</v>
       </c>
       <c r="G43" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B44" s="2">
-        <v>45474</v>
+        <v>45261</v>
       </c>
       <c r="C44" s="2">
-        <v>45504</v>
+        <v>45291</v>
       </c>
       <c r="D44">
-        <v>-808.95</v>
+        <v>22000</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>23580</v>
       </c>
       <c r="F44">
-        <v>1617.96</v>
+        <v>23580</v>
       </c>
       <c r="G44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B45" s="2">
-        <v>45505</v>
+        <v>45536</v>
       </c>
       <c r="C45" s="2">
-        <v>45535</v>
+        <v>45565</v>
       </c>
       <c r="D45">
-        <v>-808.95</v>
+        <v>-23746.8</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>28918.2</v>
       </c>
       <c r="F45">
-        <v>809.0099999999998</v>
+        <v>28918.2</v>
       </c>
       <c r="G45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B46" s="2">
-        <v>45444</v>
+        <v>45566</v>
       </c>
       <c r="C46" s="2">
-        <v>45473</v>
+        <v>45596</v>
       </c>
       <c r="D46">
-        <v>-500</v>
+        <v>3426.280000000002</v>
       </c>
       <c r="E46">
-        <v>3627.74</v>
+        <v>0</v>
       </c>
       <c r="F46">
-        <v>3627.74</v>
+        <v>32344.48</v>
       </c>
       <c r="G46" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B47" s="2">
-        <v>45474</v>
+        <v>45536</v>
       </c>
       <c r="C47" s="2">
-        <v>45504</v>
+        <v>45565</v>
       </c>
       <c r="D47">
-        <v>-248</v>
+        <v>0.23</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>28247.6</v>
       </c>
       <c r="F47">
-        <v>3379.74</v>
+        <v>28247.6</v>
       </c>
       <c r="G47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B48" s="2">
-        <v>45444</v>
+        <v>45566</v>
       </c>
       <c r="C48" s="2">
-        <v>45473</v>
+        <v>45596</v>
       </c>
       <c r="D48">
-        <v>990.96</v>
+        <v>0.24</v>
       </c>
       <c r="E48">
-        <v>9564.49</v>
+        <v>0</v>
       </c>
       <c r="F48">
-        <v>9564.49</v>
+        <v>28247.84</v>
       </c>
       <c r="G48" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B49" s="2">
-        <v>45474</v>
+        <v>45536</v>
       </c>
       <c r="C49" s="2">
-        <v>45504</v>
+        <v>45565</v>
       </c>
       <c r="D49">
-        <v>1256.21</v>
+        <v>-1779.04</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>139378.76</v>
       </c>
       <c r="F49">
-        <v>10820.7</v>
+        <v>139378.76</v>
       </c>
       <c r="G49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B50" s="2">
-        <v>45505</v>
+        <v>45566</v>
       </c>
       <c r="C50" s="2">
-        <v>45535</v>
+        <v>45596</v>
       </c>
       <c r="D50">
-        <v>-843.79</v>
+        <v>119.61</v>
       </c>
       <c r="E50">
         <v>0</v>
       </c>
       <c r="F50">
-        <v>9976.91</v>
+        <v>139498.37</v>
       </c>
       <c r="G50" t="s">
         <v>35</v>
@@ -1641,22 +1641,22 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B51" s="2">
-        <v>45444</v>
+        <v>44866</v>
       </c>
       <c r="C51" s="2">
-        <v>45473</v>
+        <v>44895</v>
       </c>
       <c r="D51">
-        <v>776.2</v>
+        <v>-900</v>
       </c>
       <c r="E51">
-        <v>9469.17</v>
+        <v>5450</v>
       </c>
       <c r="F51">
-        <v>9469.17</v>
+        <v>5450</v>
       </c>
       <c r="G51" t="s">
         <v>34</v>
@@ -1664,323 +1664,24 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B52" s="2">
-        <v>45474</v>
+        <v>44896</v>
       </c>
       <c r="C52" s="2">
-        <v>45504</v>
+        <v>44926</v>
       </c>
       <c r="D52">
-        <v>1130.99</v>
+        <v>2500</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>3700</v>
       </c>
       <c r="F52">
-        <v>10600.16</v>
+        <v>3700</v>
       </c>
       <c r="G52" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
-      <c r="A53" t="s">
-        <v>26</v>
-      </c>
-      <c r="B53" s="2">
-        <v>45505</v>
-      </c>
-      <c r="C53" s="2">
-        <v>45535</v>
-      </c>
-      <c r="D53">
-        <v>-769.01</v>
-      </c>
-      <c r="E53">
-        <v>0</v>
-      </c>
-      <c r="F53">
-        <v>9831.15</v>
-      </c>
-      <c r="G53" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
-      <c r="A54" t="s">
-        <v>27</v>
-      </c>
-      <c r="B54" s="2">
-        <v>45444</v>
-      </c>
-      <c r="C54" s="2">
-        <v>45473</v>
-      </c>
-      <c r="D54">
-        <v>500</v>
-      </c>
-      <c r="E54">
-        <v>446.48</v>
-      </c>
-      <c r="F54">
-        <v>446.48</v>
-      </c>
-      <c r="G54" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="A55" t="s">
-        <v>27</v>
-      </c>
-      <c r="B55" s="2">
-        <v>45474</v>
-      </c>
-      <c r="C55" s="2">
-        <v>45504</v>
-      </c>
-      <c r="D55">
-        <v>43.32000000000001</v>
-      </c>
-      <c r="E55">
-        <v>0</v>
-      </c>
-      <c r="F55">
-        <v>489.8</v>
-      </c>
-      <c r="G55" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
-      <c r="A56" t="s">
-        <v>28</v>
-      </c>
-      <c r="B56" s="2">
-        <v>45261</v>
-      </c>
-      <c r="C56" s="2">
-        <v>45291</v>
-      </c>
-      <c r="D56">
-        <v>22000</v>
-      </c>
-      <c r="E56">
-        <v>23580</v>
-      </c>
-      <c r="F56">
-        <v>23580</v>
-      </c>
-      <c r="G56" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
-      <c r="A57" t="s">
-        <v>29</v>
-      </c>
-      <c r="B57" s="2">
-        <v>45444</v>
-      </c>
-      <c r="C57" s="2">
-        <v>45473</v>
-      </c>
-      <c r="D57">
-        <v>11532.51</v>
-      </c>
-      <c r="E57">
-        <v>40836.43</v>
-      </c>
-      <c r="F57">
-        <v>40836.43</v>
-      </c>
-      <c r="G57" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
-      <c r="A58" t="s">
-        <v>29</v>
-      </c>
-      <c r="B58" s="2">
-        <v>45474</v>
-      </c>
-      <c r="C58" s="2">
-        <v>45504</v>
-      </c>
-      <c r="D58">
-        <v>4908.370000000002</v>
-      </c>
-      <c r="E58">
-        <v>0</v>
-      </c>
-      <c r="F58">
-        <v>45744.8</v>
-      </c>
-      <c r="G58" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
-      <c r="A59" t="s">
-        <v>29</v>
-      </c>
-      <c r="B59" s="2">
-        <v>45505</v>
-      </c>
-      <c r="C59" s="2">
-        <v>45535</v>
-      </c>
-      <c r="D59">
-        <v>-1500</v>
-      </c>
-      <c r="E59">
-        <v>0</v>
-      </c>
-      <c r="F59">
-        <v>44244.8</v>
-      </c>
-      <c r="G59" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="A60" t="s">
-        <v>30</v>
-      </c>
-      <c r="B60" s="2">
-        <v>45444</v>
-      </c>
-      <c r="C60" s="2">
-        <v>45473</v>
-      </c>
-      <c r="D60">
-        <v>0.24</v>
-      </c>
-      <c r="E60">
-        <v>28246.89</v>
-      </c>
-      <c r="F60">
-        <v>28246.89</v>
-      </c>
-      <c r="G60" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
-      <c r="A61" t="s">
-        <v>30</v>
-      </c>
-      <c r="B61" s="2">
-        <v>45474</v>
-      </c>
-      <c r="C61" s="2">
-        <v>45504</v>
-      </c>
-      <c r="D61">
-        <v>0.24</v>
-      </c>
-      <c r="E61">
-        <v>0</v>
-      </c>
-      <c r="F61">
-        <v>28247.13</v>
-      </c>
-      <c r="G61" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62" t="s">
-        <v>31</v>
-      </c>
-      <c r="B62" s="2">
-        <v>45444</v>
-      </c>
-      <c r="C62" s="2">
-        <v>45473</v>
-      </c>
-      <c r="D62">
-        <v>-100493.58</v>
-      </c>
-      <c r="E62">
-        <v>290764.34</v>
-      </c>
-      <c r="F62">
-        <v>290764.34</v>
-      </c>
-      <c r="G62" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="A63" t="s">
-        <v>31</v>
-      </c>
-      <c r="B63" s="2">
-        <v>45474</v>
-      </c>
-      <c r="C63" s="2">
-        <v>45504</v>
-      </c>
-      <c r="D63">
-        <v>-148781.23</v>
-      </c>
-      <c r="E63">
-        <v>0</v>
-      </c>
-      <c r="F63">
-        <v>141983.11</v>
-      </c>
-      <c r="G63" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64" t="s">
-        <v>32</v>
-      </c>
-      <c r="B64" s="2">
-        <v>44866</v>
-      </c>
-      <c r="C64" s="2">
-        <v>44895</v>
-      </c>
-      <c r="D64">
-        <v>-900</v>
-      </c>
-      <c r="E64">
-        <v>5450</v>
-      </c>
-      <c r="F64">
-        <v>5450</v>
-      </c>
-      <c r="G64" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
-      <c r="A65" t="s">
-        <v>33</v>
-      </c>
-      <c r="B65" s="2">
-        <v>44896</v>
-      </c>
-      <c r="C65" s="2">
-        <v>44926</v>
-      </c>
-      <c r="D65">
-        <v>2500</v>
-      </c>
-      <c r="E65">
-        <v>3700</v>
-      </c>
-      <c r="F65">
-        <v>3700</v>
-      </c>
-      <c r="G65" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Initialize Vite project with React and TypeScript setup, including configuration files, main application structure, and API client setup.
</commit_message>
<xml_diff>
--- a/STEP6Calculated Cashflows.xlsx
+++ b/STEP6Calculated Cashflows.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="36">
   <si>
     <t>bank_account_key</t>
   </si>
@@ -483,7 +483,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -517,19 +517,19 @@
         <v>7</v>
       </c>
       <c r="B2" s="2">
-        <v>45536</v>
+        <v>45566</v>
       </c>
       <c r="C2" s="2">
-        <v>45565</v>
+        <v>45596</v>
       </c>
       <c r="D2">
-        <v>1144.8</v>
+        <v>1169.8</v>
       </c>
       <c r="E2">
-        <v>10383.79</v>
+        <v>11553.59</v>
       </c>
       <c r="F2">
-        <v>10383.79</v>
+        <v>11553.59</v>
       </c>
       <c r="G2" t="s">
         <v>34</v>
@@ -540,19 +540,19 @@
         <v>7</v>
       </c>
       <c r="B3" s="2">
-        <v>45566</v>
+        <v>45597</v>
       </c>
       <c r="C3" s="2">
-        <v>45596</v>
+        <v>45626</v>
       </c>
       <c r="D3">
-        <v>1169.8</v>
+        <v>-805.2</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>11553.59</v>
+        <v>10748.39</v>
       </c>
       <c r="G3" t="s">
         <v>35</v>
@@ -560,25 +560,25 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2">
-        <v>45536</v>
+        <v>45627</v>
       </c>
       <c r="C4" s="2">
-        <v>45565</v>
+        <v>45657</v>
       </c>
       <c r="D4">
-        <v>-772.88</v>
+        <v>-9380.129999999999</v>
       </c>
       <c r="E4">
-        <v>4796.49</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>4796.49</v>
+        <v>1368.26</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -595,56 +595,56 @@
         <v>554.88</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>5351.37</v>
       </c>
       <c r="F5">
         <v>5351.37</v>
       </c>
       <c r="G5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>45536</v>
+        <v>45597</v>
       </c>
       <c r="C6" s="2">
-        <v>45565</v>
+        <v>45626</v>
       </c>
       <c r="D6">
-        <v>1223.03</v>
+        <v>-823.9299999999999</v>
       </c>
       <c r="E6">
-        <v>10017.96</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>10017.96</v>
+        <v>4527.44</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
-        <v>45566</v>
+        <v>45627</v>
       </c>
       <c r="C7" s="2">
-        <v>45596</v>
+        <v>45657</v>
       </c>
       <c r="D7">
-        <v>1223.03</v>
+        <v>-2968.08</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>11240.99</v>
+        <v>1559.36</v>
       </c>
       <c r="G7" t="s">
         <v>35</v>
@@ -652,22 +652,22 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2">
-        <v>45536</v>
+        <v>45566</v>
       </c>
       <c r="C8" s="2">
-        <v>45565</v>
+        <v>45596</v>
       </c>
       <c r="D8">
-        <v>98.52</v>
+        <v>1223.03</v>
       </c>
       <c r="E8">
-        <v>6543.22</v>
+        <v>11240.99</v>
       </c>
       <c r="F8">
-        <v>6543.22</v>
+        <v>11240.99</v>
       </c>
       <c r="G8" t="s">
         <v>34</v>
@@ -675,22 +675,22 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>45566</v>
+        <v>45597</v>
       </c>
       <c r="C9" s="2">
-        <v>45596</v>
+        <v>45626</v>
       </c>
       <c r="D9">
-        <v>1972.52</v>
+        <v>1223.03</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>8515.74</v>
+        <v>12464.02</v>
       </c>
       <c r="G9" t="s">
         <v>35</v>
@@ -698,30 +698,30 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>45536</v>
+        <v>45627</v>
       </c>
       <c r="C10" s="2">
-        <v>45565</v>
+        <v>45657</v>
       </c>
       <c r="D10">
-        <v>1134.37</v>
+        <v>-11317.04</v>
       </c>
       <c r="E10">
-        <v>9254.049999999999</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>9254.049999999999</v>
+        <v>1146.98</v>
       </c>
       <c r="G10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2">
         <v>45566</v>
@@ -730,21 +730,21 @@
         <v>45596</v>
       </c>
       <c r="D11">
-        <v>181.73</v>
+        <v>1972.52</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>8515.74</v>
       </c>
       <c r="F11">
-        <v>9435.779999999999</v>
+        <v>8515.74</v>
       </c>
       <c r="G11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>45597</v>
@@ -753,13 +753,13 @@
         <v>45626</v>
       </c>
       <c r="D12">
-        <v>-675.63</v>
+        <v>-786.48</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>8760.15</v>
+        <v>7729.26</v>
       </c>
       <c r="G12" t="s">
         <v>35</v>
@@ -767,30 +767,30 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="2">
-        <v>45536</v>
+        <v>45627</v>
       </c>
       <c r="C13" s="2">
-        <v>45565</v>
+        <v>45657</v>
       </c>
       <c r="D13">
-        <v>1218.98</v>
+        <v>-5997.4</v>
       </c>
       <c r="E13">
-        <v>10537.9</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>10537.9</v>
+        <v>1731.860000000001</v>
       </c>
       <c r="G13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="2">
         <v>45566</v>
@@ -799,59 +799,59 @@
         <v>45596</v>
       </c>
       <c r="D14">
-        <v>1218.98</v>
+        <v>181.73</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>9435.780000000001</v>
       </c>
       <c r="F14">
-        <v>11756.88</v>
+        <v>9435.780000000001</v>
       </c>
       <c r="G14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" s="2">
-        <v>45536</v>
+        <v>45597</v>
       </c>
       <c r="C15" s="2">
-        <v>45565</v>
+        <v>45626</v>
       </c>
       <c r="D15">
-        <v>150.03</v>
+        <v>1134.37</v>
       </c>
       <c r="E15">
-        <v>3261.52</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>3261.52</v>
+        <v>10570.15</v>
       </c>
       <c r="G15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" s="2">
-        <v>45566</v>
+        <v>45627</v>
       </c>
       <c r="C16" s="2">
-        <v>45596</v>
+        <v>45657</v>
       </c>
       <c r="D16">
-        <v>150.03</v>
+        <v>-9229.41</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>3411.55</v>
+        <v>1340.740000000002</v>
       </c>
       <c r="G16" t="s">
         <v>35</v>
@@ -859,22 +859,22 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17" s="2">
-        <v>45536</v>
+        <v>45566</v>
       </c>
       <c r="C17" s="2">
-        <v>45565</v>
+        <v>45596</v>
       </c>
       <c r="D17">
-        <v>-1444.66</v>
+        <v>1218.98</v>
       </c>
       <c r="E17">
-        <v>15261.69</v>
+        <v>11756.88</v>
       </c>
       <c r="F17">
-        <v>15261.69</v>
+        <v>11756.88</v>
       </c>
       <c r="G17" t="s">
         <v>34</v>
@@ -882,22 +882,22 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B18" s="2">
-        <v>45566</v>
+        <v>45597</v>
       </c>
       <c r="C18" s="2">
-        <v>45596</v>
+        <v>45626</v>
       </c>
       <c r="D18">
-        <v>3856.25</v>
+        <v>1068.98</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>19117.94</v>
+        <v>12825.86</v>
       </c>
       <c r="G18" t="s">
         <v>35</v>
@@ -905,30 +905,30 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B19" s="2">
-        <v>45536</v>
+        <v>45627</v>
       </c>
       <c r="C19" s="2">
-        <v>45565</v>
+        <v>45657</v>
       </c>
       <c r="D19">
-        <v>2651.62</v>
+        <v>-11325.64</v>
       </c>
       <c r="E19">
-        <v>12931.56</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>12931.56</v>
+        <v>1500.219999999999</v>
       </c>
       <c r="G19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B20" s="2">
         <v>45566</v>
@@ -937,67 +937,67 @@
         <v>45596</v>
       </c>
       <c r="D20">
-        <v>-38.38</v>
+        <v>150.03</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>3411.55</v>
       </c>
       <c r="F20">
-        <v>12893.18</v>
+        <v>3411.55</v>
       </c>
       <c r="G20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B21" s="2">
-        <v>45536</v>
+        <v>45597</v>
       </c>
       <c r="C21" s="2">
-        <v>45565</v>
+        <v>45626</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>150.03</v>
       </c>
       <c r="E21">
-        <v>1965.73</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>1965.73</v>
+        <v>3561.58</v>
       </c>
       <c r="G21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B22" s="2">
-        <v>45536</v>
+        <v>45627</v>
       </c>
       <c r="C22" s="2">
-        <v>45565</v>
+        <v>45657</v>
       </c>
       <c r="D22">
-        <v>0.02</v>
+        <v>-2349.97</v>
       </c>
       <c r="E22">
-        <v>1723.5</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>1723.5</v>
+        <v>1211.610000000001</v>
       </c>
       <c r="G22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B23" s="2">
         <v>45566</v>
@@ -1006,67 +1006,67 @@
         <v>45596</v>
       </c>
       <c r="D23">
-        <v>0.01</v>
+        <v>3856.25</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>19117.94</v>
       </c>
       <c r="F23">
-        <v>1723.51</v>
+        <v>19117.94</v>
       </c>
       <c r="G23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B24" s="2">
-        <v>45139</v>
+        <v>45597</v>
       </c>
       <c r="C24" s="2">
-        <v>45169</v>
+        <v>45626</v>
       </c>
       <c r="D24">
-        <v>-900</v>
+        <v>2983.84</v>
       </c>
       <c r="E24">
-        <v>7579.48</v>
+        <v>0</v>
       </c>
       <c r="F24">
-        <v>7579.48</v>
+        <v>22101.78</v>
       </c>
       <c r="G24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B25" s="2">
-        <v>45536</v>
+        <v>45627</v>
       </c>
       <c r="C25" s="2">
-        <v>45565</v>
+        <v>45657</v>
       </c>
       <c r="D25">
-        <v>1602.39</v>
+        <v>-20236.13</v>
       </c>
       <c r="E25">
-        <v>13971.89</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>13971.89</v>
+        <v>1865.649999999998</v>
       </c>
       <c r="G25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B26" s="2">
         <v>45566</v>
@@ -1075,59 +1075,59 @@
         <v>45596</v>
       </c>
       <c r="D26">
-        <v>1597.41</v>
+        <v>-38.38</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>12893.18</v>
       </c>
       <c r="F26">
-        <v>15569.3</v>
+        <v>12893.18</v>
       </c>
       <c r="G26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B27" s="2">
-        <v>45536</v>
+        <v>45597</v>
       </c>
       <c r="C27" s="2">
-        <v>45565</v>
+        <v>45626</v>
       </c>
       <c r="D27">
-        <v>7432.61</v>
+        <v>1306.62</v>
       </c>
       <c r="E27">
-        <v>25902.29</v>
+        <v>0</v>
       </c>
       <c r="F27">
-        <v>25902.29</v>
+        <v>14199.8</v>
       </c>
       <c r="G27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B28" s="2">
-        <v>45566</v>
+        <v>45627</v>
       </c>
       <c r="C28" s="2">
-        <v>45596</v>
+        <v>45657</v>
       </c>
       <c r="D28">
-        <v>379.0700000000001</v>
+        <v>-13041.2</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>26281.36</v>
+        <v>1158.6</v>
       </c>
       <c r="G28" t="s">
         <v>35</v>
@@ -1135,7 +1135,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B29" s="2">
         <v>45536</v>
@@ -1144,13 +1144,13 @@
         <v>45565</v>
       </c>
       <c r="D29">
-        <v>2237.59</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>16890.32</v>
+        <v>1965.73</v>
       </c>
       <c r="F29">
-        <v>16890.32</v>
+        <v>1965.73</v>
       </c>
       <c r="G29" t="s">
         <v>34</v>
@@ -1158,22 +1158,22 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B30" s="2">
-        <v>45566</v>
+        <v>45597</v>
       </c>
       <c r="C30" s="2">
-        <v>45596</v>
+        <v>45626</v>
       </c>
       <c r="D30">
-        <v>65.98000000000002</v>
+        <v>0</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30">
-        <v>16956.3</v>
+        <v>1965.73</v>
       </c>
       <c r="G30" t="s">
         <v>35</v>
@@ -1181,22 +1181,22 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B31" s="2">
-        <v>45597</v>
+        <v>45627</v>
       </c>
       <c r="C31" s="2">
-        <v>45626</v>
+        <v>45657</v>
       </c>
       <c r="D31">
-        <v>-1383.06</v>
+        <v>0</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="F31">
-        <v>15573.24</v>
+        <v>1965.73</v>
       </c>
       <c r="G31" t="s">
         <v>35</v>
@@ -1204,22 +1204,22 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B32" s="2">
-        <v>45536</v>
+        <v>45566</v>
       </c>
       <c r="C32" s="2">
-        <v>45565</v>
+        <v>45596</v>
       </c>
       <c r="D32">
-        <v>181.94</v>
+        <v>0.01</v>
       </c>
       <c r="E32">
-        <v>9722.58</v>
+        <v>1723.51</v>
       </c>
       <c r="F32">
-        <v>9722.58</v>
+        <v>1723.51</v>
       </c>
       <c r="G32" t="s">
         <v>34</v>
@@ -1227,22 +1227,22 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B33" s="2">
-        <v>45566</v>
+        <v>45597</v>
       </c>
       <c r="C33" s="2">
-        <v>45596</v>
+        <v>45626</v>
       </c>
       <c r="D33">
-        <v>2376.55</v>
+        <v>0.02</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
       <c r="F33">
-        <v>12099.13</v>
+        <v>1723.53</v>
       </c>
       <c r="G33" t="s">
         <v>35</v>
@@ -1250,22 +1250,22 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B34" s="2">
-        <v>45597</v>
+        <v>45627</v>
       </c>
       <c r="C34" s="2">
-        <v>45626</v>
+        <v>45657</v>
       </c>
       <c r="D34">
-        <v>-1383.06</v>
+        <v>0.01000000000021828</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34">
-        <v>10716.07</v>
+        <v>1723.54</v>
       </c>
       <c r="G34" t="s">
         <v>35</v>
@@ -1273,22 +1273,22 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B35" s="2">
-        <v>45536</v>
+        <v>45139</v>
       </c>
       <c r="C35" s="2">
-        <v>45565</v>
+        <v>45169</v>
       </c>
       <c r="D35">
-        <v>189.62</v>
+        <v>-900</v>
       </c>
       <c r="E35">
-        <v>998.63</v>
+        <v>7579.48</v>
       </c>
       <c r="F35">
-        <v>998.63</v>
+        <v>7579.48</v>
       </c>
       <c r="G35" t="s">
         <v>34</v>
@@ -1296,22 +1296,22 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B36" s="2">
-        <v>45566</v>
+        <v>45627</v>
       </c>
       <c r="C36" s="2">
-        <v>45596</v>
+        <v>45657</v>
       </c>
       <c r="D36">
-        <v>-808.95</v>
+        <v>-5683.63</v>
       </c>
       <c r="E36">
         <v>0</v>
       </c>
       <c r="F36">
-        <v>189.6799999999999</v>
+        <v>1895.849999999999</v>
       </c>
       <c r="G36" t="s">
         <v>35</v>
@@ -1319,22 +1319,22 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B37" s="2">
-        <v>45474</v>
+        <v>45566</v>
       </c>
       <c r="C37" s="2">
-        <v>45504</v>
+        <v>45596</v>
       </c>
       <c r="D37">
-        <v>-248</v>
+        <v>1597.41</v>
       </c>
       <c r="E37">
-        <v>3379.74</v>
+        <v>15569.3</v>
       </c>
       <c r="F37">
-        <v>3379.74</v>
+        <v>15569.3</v>
       </c>
       <c r="G37" t="s">
         <v>34</v>
@@ -1342,45 +1342,45 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B38" s="2">
-        <v>45536</v>
+        <v>45597</v>
       </c>
       <c r="C38" s="2">
-        <v>45565</v>
+        <v>45626</v>
       </c>
       <c r="D38">
-        <v>-630.79</v>
+        <v>-306.6</v>
       </c>
       <c r="E38">
-        <v>11160.5</v>
+        <v>0</v>
       </c>
       <c r="F38">
-        <v>11160.5</v>
+        <v>15262.7</v>
       </c>
       <c r="G38" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B39" s="2">
-        <v>45566</v>
+        <v>45627</v>
       </c>
       <c r="C39" s="2">
-        <v>45596</v>
+        <v>45657</v>
       </c>
       <c r="D39">
-        <v>1306.21</v>
+        <v>-13556.85</v>
       </c>
       <c r="E39">
         <v>0</v>
       </c>
       <c r="F39">
-        <v>12466.71</v>
+        <v>1705.849999999999</v>
       </c>
       <c r="G39" t="s">
         <v>35</v>
@@ -1388,22 +1388,22 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B40" s="2">
-        <v>45536</v>
+        <v>45566</v>
       </c>
       <c r="C40" s="2">
-        <v>45565</v>
+        <v>45596</v>
       </c>
       <c r="D40">
-        <v>940.99</v>
+        <v>379.07</v>
       </c>
       <c r="E40">
-        <v>12672.14</v>
+        <v>26281.36</v>
       </c>
       <c r="F40">
-        <v>12672.14</v>
+        <v>26281.36</v>
       </c>
       <c r="G40" t="s">
         <v>34</v>
@@ -1411,22 +1411,22 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B41" s="2">
-        <v>45566</v>
+        <v>45597</v>
       </c>
       <c r="C41" s="2">
-        <v>45596</v>
+        <v>45626</v>
       </c>
       <c r="D41">
-        <v>1230.99</v>
+        <v>1453.71</v>
       </c>
       <c r="E41">
         <v>0</v>
       </c>
       <c r="F41">
-        <v>13903.13</v>
+        <v>27735.07</v>
       </c>
       <c r="G41" t="s">
         <v>35</v>
@@ -1434,30 +1434,30 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B42" s="2">
-        <v>45536</v>
+        <v>45627</v>
       </c>
       <c r="C42" s="2">
-        <v>45565</v>
+        <v>45657</v>
       </c>
       <c r="D42">
-        <v>-71.53</v>
+        <v>-25478.64</v>
       </c>
       <c r="E42">
-        <v>377.92</v>
+        <v>0</v>
       </c>
       <c r="F42">
-        <v>377.92</v>
+        <v>2256.43</v>
       </c>
       <c r="G42" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B43" s="2">
         <v>45566</v>
@@ -1466,67 +1466,67 @@
         <v>45596</v>
       </c>
       <c r="D43">
-        <v>-28.17</v>
+        <v>65.98</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>16956.3</v>
       </c>
       <c r="F43">
-        <v>349.75</v>
+        <v>16956.3</v>
       </c>
       <c r="G43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B44" s="2">
-        <v>45261</v>
+        <v>45597</v>
       </c>
       <c r="C44" s="2">
-        <v>45291</v>
+        <v>45626</v>
       </c>
       <c r="D44">
-        <v>22000</v>
+        <v>1441.94</v>
       </c>
       <c r="E44">
-        <v>23580</v>
+        <v>0</v>
       </c>
       <c r="F44">
-        <v>23580</v>
+        <v>18398.24</v>
       </c>
       <c r="G44" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B45" s="2">
-        <v>45536</v>
+        <v>45627</v>
       </c>
       <c r="C45" s="2">
-        <v>45565</v>
+        <v>45657</v>
       </c>
       <c r="D45">
-        <v>-23746.8</v>
+        <v>-16841.48</v>
       </c>
       <c r="E45">
-        <v>28918.2</v>
+        <v>0</v>
       </c>
       <c r="F45">
-        <v>28918.2</v>
+        <v>1556.759999999998</v>
       </c>
       <c r="G45" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B46" s="2">
         <v>45566</v>
@@ -1535,59 +1535,59 @@
         <v>45596</v>
       </c>
       <c r="D46">
-        <v>3426.280000000002</v>
+        <v>2376.55</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <v>12099.13</v>
       </c>
       <c r="F46">
-        <v>32344.48</v>
+        <v>12099.13</v>
       </c>
       <c r="G46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B47" s="2">
-        <v>45536</v>
+        <v>45597</v>
       </c>
       <c r="C47" s="2">
-        <v>45565</v>
+        <v>45626</v>
       </c>
       <c r="D47">
-        <v>0.23</v>
+        <v>3174.94</v>
       </c>
       <c r="E47">
-        <v>28247.6</v>
+        <v>0</v>
       </c>
       <c r="F47">
-        <v>28247.6</v>
+        <v>15274.07</v>
       </c>
       <c r="G47" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B48" s="2">
-        <v>45566</v>
+        <v>45627</v>
       </c>
       <c r="C48" s="2">
-        <v>45596</v>
+        <v>45657</v>
       </c>
       <c r="D48">
-        <v>0.24</v>
+        <v>-12968.77</v>
       </c>
       <c r="E48">
         <v>0</v>
       </c>
       <c r="F48">
-        <v>28247.84</v>
+        <v>2305.300000000001</v>
       </c>
       <c r="G48" t="s">
         <v>35</v>
@@ -1595,22 +1595,22 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B49" s="2">
-        <v>45536</v>
+        <v>45566</v>
       </c>
       <c r="C49" s="2">
-        <v>45565</v>
+        <v>45596</v>
       </c>
       <c r="D49">
-        <v>-1779.04</v>
+        <v>-808.95</v>
       </c>
       <c r="E49">
-        <v>139378.76</v>
+        <v>189.68</v>
       </c>
       <c r="F49">
-        <v>139378.76</v>
+        <v>189.68</v>
       </c>
       <c r="G49" t="s">
         <v>34</v>
@@ -1618,22 +1618,22 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B50" s="2">
-        <v>45566</v>
+        <v>45597</v>
       </c>
       <c r="C50" s="2">
-        <v>45596</v>
+        <v>45626</v>
       </c>
       <c r="D50">
-        <v>119.61</v>
+        <v>3191.05</v>
       </c>
       <c r="E50">
         <v>0</v>
       </c>
       <c r="F50">
-        <v>139498.37</v>
+        <v>3380.73</v>
       </c>
       <c r="G50" t="s">
         <v>35</v>
@@ -1641,47 +1641,576 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B51" s="2">
-        <v>44866</v>
+        <v>45627</v>
       </c>
       <c r="C51" s="2">
-        <v>44895</v>
+        <v>45657</v>
       </c>
       <c r="D51">
-        <v>-900</v>
+        <v>-1688.33</v>
       </c>
       <c r="E51">
-        <v>5450</v>
+        <v>0</v>
       </c>
       <c r="F51">
-        <v>5450</v>
+        <v>1692.4</v>
       </c>
       <c r="G51" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
+        <v>24</v>
+      </c>
+      <c r="B52" s="2">
+        <v>45474</v>
+      </c>
+      <c r="C52" s="2">
+        <v>45504</v>
+      </c>
+      <c r="D52">
+        <v>-248</v>
+      </c>
+      <c r="E52">
+        <v>3379.74</v>
+      </c>
+      <c r="F52">
+        <v>3379.74</v>
+      </c>
+      <c r="G52" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" s="2">
+        <v>45566</v>
+      </c>
+      <c r="C53" s="2">
+        <v>45596</v>
+      </c>
+      <c r="D53">
+        <v>1306.21</v>
+      </c>
+      <c r="E53">
+        <v>12466.71</v>
+      </c>
+      <c r="F53">
+        <v>12466.71</v>
+      </c>
+      <c r="G53" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54" s="2">
+        <v>45597</v>
+      </c>
+      <c r="C54" s="2">
+        <v>45626</v>
+      </c>
+      <c r="D54">
+        <v>1156.21</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>13622.92</v>
+      </c>
+      <c r="G54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" s="2">
+        <v>45627</v>
+      </c>
+      <c r="C55" s="2">
+        <v>45657</v>
+      </c>
+      <c r="D55">
+        <v>-11614.19</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>2008.729999999998</v>
+      </c>
+      <c r="G55" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" s="2">
+        <v>45658</v>
+      </c>
+      <c r="C56" s="2">
+        <v>45688</v>
+      </c>
+      <c r="D56">
+        <v>-75</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>1933.729999999998</v>
+      </c>
+      <c r="G56" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" s="2">
+        <v>45566</v>
+      </c>
+      <c r="C57" s="2">
+        <v>45596</v>
+      </c>
+      <c r="D57">
+        <v>1230.99</v>
+      </c>
+      <c r="E57">
+        <v>13903.13</v>
+      </c>
+      <c r="F57">
+        <v>13903.13</v>
+      </c>
+      <c r="G57" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" s="2">
+        <v>45597</v>
+      </c>
+      <c r="C58" s="2">
+        <v>45626</v>
+      </c>
+      <c r="D58">
+        <v>1230.99</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>15134.12</v>
+      </c>
+      <c r="G58" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" s="2">
+        <v>45627</v>
+      </c>
+      <c r="C59" s="2">
+        <v>45657</v>
+      </c>
+      <c r="D59">
+        <v>-13243.3</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>1890.82</v>
+      </c>
+      <c r="G59" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" t="s">
+        <v>27</v>
+      </c>
+      <c r="B60" s="2">
+        <v>45566</v>
+      </c>
+      <c r="C60" s="2">
+        <v>45596</v>
+      </c>
+      <c r="D60">
+        <v>-28.17</v>
+      </c>
+      <c r="E60">
+        <v>349.75</v>
+      </c>
+      <c r="F60">
+        <v>349.75</v>
+      </c>
+      <c r="G60" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" s="2">
+        <v>45597</v>
+      </c>
+      <c r="C61" s="2">
+        <v>45626</v>
+      </c>
+      <c r="D61">
+        <v>-28.22</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>321.53</v>
+      </c>
+      <c r="G61" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62" s="2">
+        <v>45627</v>
+      </c>
+      <c r="C62" s="2">
+        <v>45657</v>
+      </c>
+      <c r="D62">
+        <v>-41.69</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>279.84</v>
+      </c>
+      <c r="G62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" t="s">
+        <v>28</v>
+      </c>
+      <c r="B63" s="2">
+        <v>45261</v>
+      </c>
+      <c r="C63" s="2">
+        <v>45291</v>
+      </c>
+      <c r="D63">
+        <v>22000</v>
+      </c>
+      <c r="E63">
+        <v>23580</v>
+      </c>
+      <c r="F63">
+        <v>23580</v>
+      </c>
+      <c r="G63" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" t="s">
+        <v>28</v>
+      </c>
+      <c r="B64" s="2">
+        <v>45627</v>
+      </c>
+      <c r="C64" s="2">
+        <v>45657</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>23580</v>
+      </c>
+      <c r="G64" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" t="s">
+        <v>29</v>
+      </c>
+      <c r="B65" s="2">
+        <v>45566</v>
+      </c>
+      <c r="C65" s="2">
+        <v>45596</v>
+      </c>
+      <c r="D65">
+        <v>3426.28</v>
+      </c>
+      <c r="E65">
+        <v>32344.48</v>
+      </c>
+      <c r="F65">
+        <v>32344.48</v>
+      </c>
+      <c r="G65" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" t="s">
+        <v>29</v>
+      </c>
+      <c r="B66" s="2">
+        <v>45597</v>
+      </c>
+      <c r="C66" s="2">
+        <v>45626</v>
+      </c>
+      <c r="D66">
+        <v>-15221.75</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>17122.73</v>
+      </c>
+      <c r="G66" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" t="s">
+        <v>29</v>
+      </c>
+      <c r="B67" s="2">
+        <v>45627</v>
+      </c>
+      <c r="C67" s="2">
+        <v>45657</v>
+      </c>
+      <c r="D67">
+        <v>3101.199999999997</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>20223.93</v>
+      </c>
+      <c r="G67" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" t="s">
+        <v>30</v>
+      </c>
+      <c r="B68" s="2">
+        <v>45566</v>
+      </c>
+      <c r="C68" s="2">
+        <v>45596</v>
+      </c>
+      <c r="D68">
+        <v>0.24</v>
+      </c>
+      <c r="E68">
+        <v>28247.84</v>
+      </c>
+      <c r="F68">
+        <v>28247.84</v>
+      </c>
+      <c r="G68" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
+        <v>30</v>
+      </c>
+      <c r="B69" s="2">
+        <v>45597</v>
+      </c>
+      <c r="C69" s="2">
+        <v>45626</v>
+      </c>
+      <c r="D69">
+        <v>0.23</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>28248.07</v>
+      </c>
+      <c r="G69" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70" s="2">
+        <v>45627</v>
+      </c>
+      <c r="C70" s="2">
+        <v>45657</v>
+      </c>
+      <c r="D70">
+        <v>10000.24</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>38248.31</v>
+      </c>
+      <c r="G70" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" t="s">
+        <v>31</v>
+      </c>
+      <c r="B71" s="2">
+        <v>45566</v>
+      </c>
+      <c r="C71" s="2">
+        <v>45596</v>
+      </c>
+      <c r="D71">
+        <v>119.61</v>
+      </c>
+      <c r="E71">
+        <v>139498.37</v>
+      </c>
+      <c r="F71">
+        <v>139498.37</v>
+      </c>
+      <c r="G71" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" t="s">
+        <v>31</v>
+      </c>
+      <c r="B72" s="2">
+        <v>45597</v>
+      </c>
+      <c r="C72" s="2">
+        <v>45626</v>
+      </c>
+      <c r="D72">
+        <v>-7135.15</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>132363.22</v>
+      </c>
+      <c r="G72" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" t="s">
+        <v>31</v>
+      </c>
+      <c r="B73" s="2">
+        <v>45627</v>
+      </c>
+      <c r="C73" s="2">
+        <v>45657</v>
+      </c>
+      <c r="D73">
+        <v>135377.49</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>267740.71</v>
+      </c>
+      <c r="G73" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" t="s">
+        <v>32</v>
+      </c>
+      <c r="B74" s="2">
+        <v>44866</v>
+      </c>
+      <c r="C74" s="2">
+        <v>44895</v>
+      </c>
+      <c r="D74">
+        <v>-900</v>
+      </c>
+      <c r="E74">
+        <v>5450</v>
+      </c>
+      <c r="F74">
+        <v>5450</v>
+      </c>
+      <c r="G74" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" t="s">
         <v>33</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B75" s="2">
         <v>44896</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C75" s="2">
         <v>44926</v>
       </c>
-      <c r="D52">
+      <c r="D75">
         <v>2500</v>
       </c>
-      <c r="E52">
+      <c r="E75">
         <v>3700</v>
       </c>
-      <c r="F52">
+      <c r="F75">
         <v>3700</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G75" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>